<commit_message>
Preparations for CAA talk, fix Import-Function
</commit_message>
<xml_diff>
--- a/Example_data/ex_London_cem.xlsx
+++ b/Example_data/ex_London_cem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>End</t>
   </si>
@@ -51,15 +51,9 @@
     <t>St Brides Lower</t>
   </si>
   <si>
-    <t>low socio-economic status</t>
-  </si>
-  <si>
     <t>Chlesea Old Church</t>
   </si>
   <si>
-    <t>high socio-economic status</t>
-  </si>
-  <si>
     <t>urban</t>
   </si>
   <si>
@@ -70,6 +64,21 @@
   </si>
   <si>
     <t>unkown</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>low socio- economic status</t>
+  </si>
+  <si>
+    <t>high socio- economic status</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -401,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -425,10 +434,13 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -440,12 +452,15 @@
         <v>1849</v>
       </c>
       <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -457,15 +472,18 @@
         <v>1853</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1700</v>
@@ -474,12 +492,15 @@
         <v>1850</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -491,12 +512,15 @@
         <v>1500</v>
       </c>
       <c r="E5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -508,12 +532,15 @@
         <v>1666</v>
       </c>
       <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -525,12 +552,15 @@
         <v>1666</v>
       </c>
       <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -542,12 +572,15 @@
         <v>1853</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -559,12 +592,15 @@
         <v>1666</v>
       </c>
       <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -576,15 +612,18 @@
         <v>1853</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>1569</v>
@@ -593,12 +632,15 @@
         <v>1714</v>
       </c>
       <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>17000</v>
@@ -612,10 +654,13 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>20000</v>
@@ -629,10 +674,13 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>33347</v>
@@ -646,13 +694,16 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1608</v>
@@ -663,10 +714,13 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>41313</v>
@@ -680,10 +734,13 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>11000</v>
@@ -697,10 +754,13 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>100000</v>
@@ -713,6 +773,9 @@
       </c>
       <c r="E18">
         <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +790,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -740,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>